<commit_message>
updates to writing and table added
</commit_message>
<xml_diff>
--- a/litreview/heattol_litreview.xlsx
+++ b/litreview/heattol_litreview.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicole/GitHub/heattolerance/litreview/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184686B3-8B1E-9F44-A508-18FE6F58FF32}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="780" windowWidth="34900" windowHeight="15220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="740" yWindow="560" windowWidth="11240" windowHeight="15220" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
     <sheet name="heattol_litreview" sheetId="2" r:id="rId2"/>
     <sheet name="scratch" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="152">
   <si>
     <t>Below metadata by Lizzie Wolkovich started on 29 July 2016</t>
   </si>
@@ -389,12 +395,111 @@
       <t>Good methods paper to review!</t>
     </r>
   </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Varieties</t>
+  </si>
+  <si>
+    <t>Semillon</t>
+  </si>
+  <si>
+    <t>Greer and Weston 2010</t>
+  </si>
+  <si>
+    <t>Greer and Weedon 2012</t>
+  </si>
+  <si>
+    <t>Greer and Weedon 2013</t>
+  </si>
+  <si>
+    <t>Greer and Weedon 2014</t>
+  </si>
+  <si>
+    <t>Kliewer 1968</t>
+  </si>
+  <si>
+    <t>Chardonnay, Merlot, Semillon</t>
+  </si>
+  <si>
+    <t>Cardinal, Chardonnay, Malbec, Petite Sirah, White Reisling</t>
+  </si>
+  <si>
+    <t>Kriedemann 1968</t>
+  </si>
+  <si>
+    <t>Sultana</t>
+  </si>
+  <si>
+    <t>Red Tempranillo, White Tempranillo</t>
+  </si>
+  <si>
+    <t>Hulands et al. 2013</t>
+  </si>
+  <si>
+    <t>Hulands et al. 2014</t>
+  </si>
+  <si>
+    <t>Martinez-Luscher et al. 2016</t>
+  </si>
+  <si>
+    <t>Petrie and Clingeleffer 2005</t>
+  </si>
+  <si>
+    <t>Chardonnay</t>
+  </si>
+  <si>
+    <t>Salazar Paara et al. 2010</t>
+  </si>
+  <si>
+    <t>Tempranillo</t>
+  </si>
+  <si>
+    <t>Soar et al. 2009</t>
+  </si>
+  <si>
+    <t>Shiraz</t>
+  </si>
+  <si>
+    <t>Wample et al 1991</t>
+  </si>
+  <si>
+    <t>Cabernet Sauvignon, Chardonnay, Chenin Blanc, Merlot</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>The number of flowers was siginificantly reduced by heat treatments before budburst, but not after budburst.</t>
+  </si>
+  <si>
+    <t>Max Temp (°C)</t>
+  </si>
+  <si>
+    <t>NOT IN ENDNOTE</t>
+  </si>
+  <si>
+    <t>Heat treatments later in ripening slowed ripeing to a greater degree than heat treaments earlier in berry ripening.</t>
+  </si>
+  <si>
+    <t>The rate of ripening was a curvilinear fuction of temperature, as both dry matter and sugar accumulation were affected by temperature.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flowers in plants that underwent heat treatments during flowering completely abcised.  Berry devlopment in plants treated at fruit set was not affected, but was negatively impacted when plants were treated at veraison and mid-ripening.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berries exposed to higher temperatures later in ripening suffered greater suscepability to sunburn and had smaller diameters on average than untreated plants. </t>
+  </si>
+  <si>
+    <t>Photosynthesis is optimal at 30 °C, but negatively impacted by 35 °C.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -414,6 +519,19 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -436,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -447,12 +565,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -777,12 +920,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="26" width="10.5" customWidth="1"/>
   </cols>
@@ -898,17 +1041,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="3" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="8" width="20.5" customWidth="1"/>
     <col min="9" max="27" width="10.5" customWidth="1"/>
@@ -918,7 +1062,7 @@
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -967,7 +1111,7 @@
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -995,11 +1139,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" ht="30" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1025,7 +1169,7 @@
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1055,7 +1199,7 @@
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1084,7 +1228,7 @@
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1104,11 +1248,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" ht="31" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1140,7 +1284,7 @@
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1169,7 +1313,7 @@
       <c r="A9" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -1194,11 +1338,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" ht="30" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="12" t="s">
         <v>76</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -1225,7 +1369,7 @@
       <c r="A11" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -1254,7 +1398,7 @@
       <c r="A12" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -1283,7 +1427,7 @@
       <c r="A13" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="12" t="s">
         <v>94</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -1315,7 +1459,7 @@
       <c r="A14" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="12" t="s">
         <v>112</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -9239,17 +9383,221 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="26" width="10.5" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" customHeight="1">
+      <c r="A1" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1">
+      <c r="A2" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1">
+      <c r="A3" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3">
+        <v>45</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="63" customHeight="1">
+      <c r="A4" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="130" customHeight="1">
+      <c r="A5" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="64" customHeight="1">
+      <c r="A6" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6">
+        <v>38</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="78" customHeight="1">
+      <c r="A7" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7">
+        <v>39</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" customHeight="1">
+      <c r="A8" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8">
+        <v>38</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="31" customHeight="1">
+      <c r="A9" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="31" customHeight="1">
+      <c r="A10" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="61" customHeight="1">
+      <c r="A11" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1">
+      <c r="A12" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12">
+        <v>28</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1">
+      <c r="A13" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13">
+        <v>45</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="44" customHeight="1">
+      <c r="A14" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14">
+        <v>60</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added one column to the table
</commit_message>
<xml_diff>
--- a/litreview/heattol_litreview.xlsx
+++ b/litreview/heattol_litreview.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicole/GitHub/heattolerance/litreview/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184686B3-8B1E-9F44-A508-18FE6F58FF32}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="560" windowWidth="11240" windowHeight="15220" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6020" yWindow="2000" windowWidth="34960" windowHeight="15780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
     <sheet name="heattol_litreview" sheetId="2" r:id="rId2"/>
     <sheet name="scratch" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="157">
   <si>
     <t>Below metadata by Lizzie Wolkovich started on 29 July 2016</t>
   </si>
@@ -494,12 +488,27 @@
   <si>
     <t>Photosynthesis is optimal at 30 °C, but negatively impacted by 35 °C.</t>
   </si>
+  <si>
+    <t>Phenological stage</t>
+  </si>
+  <si>
+    <t>Berry ripening</t>
+  </si>
+  <si>
+    <t>Flowering, berry ripening</t>
+  </si>
+  <si>
+    <t>Photosynthesis</t>
+  </si>
+  <si>
+    <t>Before and after budburst</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -533,6 +542,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -551,8 +572,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -583,7 +606,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -920,12 +945,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="26" width="10.5" customWidth="1"/>
   </cols>
@@ -1041,14 +1066,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="25.5" style="11" customWidth="1"/>
@@ -1455,7 +1480,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" ht="30">
       <c r="A14" s="7" t="s">
         <v>111</v>
       </c>
@@ -9383,23 +9408,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="11" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" customWidth="1"/>
-    <col min="5" max="26" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" customWidth="1"/>
+    <col min="6" max="27" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>119</v>
       </c>
@@ -9409,11 +9435,14 @@
       <c r="C1" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="14" t="s">
         <v>123</v>
       </c>
@@ -9423,11 +9452,11 @@
       <c r="C2">
         <v>40</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>124</v>
       </c>
@@ -9437,11 +9466,11 @@
       <c r="C3">
         <v>45</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="63" customHeight="1">
+    <row r="4" spans="1:5" ht="63" customHeight="1">
       <c r="A4" s="14" t="s">
         <v>125</v>
       </c>
@@ -9451,11 +9480,14 @@
       <c r="C4">
         <v>40</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="130" customHeight="1">
+    <row r="5" spans="1:5" ht="130" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>122</v>
       </c>
@@ -9465,11 +9497,14 @@
       <c r="C5">
         <v>40</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="64" customHeight="1">
+    <row r="6" spans="1:5" ht="64" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>132</v>
       </c>
@@ -9479,11 +9514,14 @@
       <c r="C6">
         <v>38</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="78" customHeight="1">
+    <row r="7" spans="1:5" ht="78" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>133</v>
       </c>
@@ -9493,11 +9531,14 @@
       <c r="C7">
         <v>39</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" customHeight="1">
+    <row r="8" spans="1:5" ht="45" customHeight="1">
       <c r="A8" s="14" t="s">
         <v>126</v>
       </c>
@@ -9507,11 +9548,11 @@
       <c r="C8">
         <v>38</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="E8" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="31" customHeight="1">
+    <row r="9" spans="1:5" ht="31" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>129</v>
       </c>
@@ -9521,11 +9562,14 @@
       <c r="C9">
         <v>50</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31" customHeight="1">
+    <row r="10" spans="1:5" ht="31" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>134</v>
       </c>
@@ -9535,11 +9579,11 @@
       <c r="C10">
         <v>30</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="E10" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="61" customHeight="1">
+    <row r="11" spans="1:5" ht="61" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>135</v>
       </c>
@@ -9549,11 +9593,14 @@
       <c r="C11">
         <v>40</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>137</v>
       </c>
@@ -9563,11 +9610,11 @@
       <c r="C12">
         <v>28</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="E12" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>139</v>
       </c>
@@ -9577,11 +9624,11 @@
       <c r="C13">
         <v>45</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="44" customHeight="1">
+    <row r="14" spans="1:5" ht="44" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>141</v>
       </c>
@@ -9591,13 +9638,13 @@
       <c r="C14">
         <v>60</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="E14" s="16" t="s">
         <v>146</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated files and new papers!
</commit_message>
<xml_diff>
--- a/litreview/heattol_litreview.xlsx
+++ b/litreview/heattol_litreview.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="166">
   <si>
     <t>Below metadata by Lizzie Wolkovich started on 29 July 2016</t>
   </si>
@@ -526,6 +526,9 @@
   </si>
   <si>
     <t>Warmer temperatures caused phenology to advance.  The effect was seen most prominently before budburst.  Between budburst and flowering the effect of higher temperatures was slightly less.  The increased temperatures had the least  effect on phenological timing between flowering and fruit set.</t>
+  </si>
+  <si>
+    <t>New studies on 19 Mar 2020 were added directly to manuscript!</t>
   </si>
 </sst>
 </file>
@@ -1005,27 +1008,27 @@
     <col min="1" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" ht="15" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -1033,7 +1036,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="15" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
@@ -1041,7 +1044,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="15" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
@@ -1049,7 +1052,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="15" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="15" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
@@ -1065,7 +1068,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="15" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="15" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="15" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1089,7 +1092,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="15" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="15" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
@@ -9461,8 +9464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -9736,7 +9739,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="61" customHeight="1"/>
+    <row r="14" spans="1:6" ht="61" customHeight="1">
+      <c r="A14" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
     <row r="15" spans="1:6" ht="49" customHeight="1"/>
     <row r="16" spans="1:6" ht="78" customHeight="1"/>
   </sheetData>

</xml_diff>